<commit_message>
Upload a valid excel file
</commit_message>
<xml_diff>
--- a/src/test/java/TestData/loginData.xlsx
+++ b/src/test/java/TestData/loginData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="26715" windowHeight="12525" activeTab="2"/>
+    <workbookView windowWidth="26715" windowHeight="12525" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Login Data" sheetId="1" r:id="rId1"/>
@@ -18,19 +18,19 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="7">
   <si>
-    <t>[HTACCESS username]</t>
+    <t>aetman</t>
   </si>
   <si>
-    <t>[HTACCESS password]</t>
+    <t>ZeeS5quuoghe5ai4taiJaRoC1ui2coh1ShahgheiMo3xiekoh6thiaThahzeZ7ei</t>
   </si>
   <si>
     <t>eg</t>
   </si>
   <si>
-    <t>[email]</t>
+    <t>ahmed.etman@jumia.com</t>
   </si>
   <si>
-    <t>[Password]</t>
+    <t>Fawryfawry@2022</t>
   </si>
   <si>
     <t>testdiscounts+new@maildrop.cc</t>
@@ -45,9 +45,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -74,8 +74,16 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -89,10 +97,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -104,6 +113,21 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
@@ -112,16 +136,23 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -129,7 +160,35 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -138,65 +197,6 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -211,187 +211,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -423,17 +423,32 @@
       <diagonal/>
     </border>
     <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF7F7F7F"/>
       </left>
       <right style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF7F7F7F"/>
       </right>
       <top style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF7F7F7F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -453,28 +468,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FFB2B2B2"/>
       </left>
       <right style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FFB2B2B2"/>
       </right>
       <top style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FFB2B2B2"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -488,17 +492,13 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
       </top>
       <bottom style="double">
-        <color rgb="FF3F3F3F"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -510,139 +510,139 @@
     <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="14" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="13" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="14" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="13" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="7" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="28" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -984,12 +984,11 @@
   <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="15.75" outlineLevelCol="4"/>
   <cols>
-    <col min="1" max="1" width="19.2222222222222" customWidth="1"/>
     <col min="2" max="2" width="62.2222222222222" customWidth="1"/>
     <col min="4" max="4" width="22.1111111111111" customWidth="1"/>
     <col min="5" max="5" width="16.1111111111111" customWidth="1"/>
@@ -1016,8 +1015,8 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D1" r:id="rId1" display="[email]"/>
-    <hyperlink ref="E1" r:id="rId2" display="[Password]" tooltip="mailto:Fawryfawry@2022"/>
+    <hyperlink ref="D1" r:id="rId1" display="ahmed.etman@jumia.com"/>
+    <hyperlink ref="E1" r:id="rId2" display="Fawryfawry@2022" tooltip="mailto:Fawryfawry@2022"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
@@ -1029,7 +1028,7 @@
   <sheetPr/>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
@@ -1056,14 +1055,13 @@
   <sheetPr/>
   <dimension ref="A1:E1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="15.75" outlineLevelCol="4"/>
   <cols>
     <col min="1" max="1" width="27.5555555555556" customWidth="1"/>
-    <col min="3" max="3" width="19.2222222222222" customWidth="1"/>
     <col min="4" max="4" width="62.2222222222222" customWidth="1"/>
     <col min="5" max="5" width="10.4444444444444" customWidth="1"/>
   </cols>

</xml_diff>